<commit_message>
Minor revisions for presentation
</commit_message>
<xml_diff>
--- a/src/main/groovy/results/CollatedResults.xlsx
+++ b/src/main/groovy/results/CollatedResults.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IJGradle\ClusterMandelbrot\src\main\groovy\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B707B378-FDDE-49A1-AB6D-94627F5A3132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1FB6024-4658-4A5D-B6CC-064E7F470A16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10" yWindow="30" windowWidth="18920" windowHeight="10550" tabRatio="945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="18770" windowHeight="9800" tabRatio="945" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="xpcTimes" sheetId="9" r:id="rId1"/>
@@ -2495,7 +2495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0EDE3E9-67F1-4C71-A85D-F86A74503BA4}">
   <dimension ref="A1:N130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N19" sqref="N19:N20"/>
     </sheetView>
   </sheetViews>
@@ -20648,8 +20648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC0A6FBD-A969-4ECF-A65F-BE420AC3BCC7}">
   <dimension ref="A1:S27"/>
   <sheetViews>
-    <sheetView zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>

</xml_diff>